<commit_message>
[webmail] - added support for [Temporary-Mail](https://temporary-mail.net) as well. - improved support and performance for [Mailinator](https://www.mailinator.com)
Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/data/unitTest_webmail.data.xlsx
+++ b/src/test/resources/unittesting/artifact/data/unitTest_webmail.data.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12495" tabRatio="500"/>
+    <workbookView windowHeight="12645" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
     <sheet name="mailinator" sheetId="3" r:id="rId2"/>
+    <sheet name="temporary-mail" sheetId="4" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
     <definedName name="base">'[1]#system'!$B$2:$B$24</definedName>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>nexial.scope.fallbackToPrevious</t>
   </si>
@@ -83,7 +84,7 @@
     <t>MyMail.from</t>
   </si>
   <si>
-    <t>johnnybgood@gmail.com</t>
+    <t>jimmyfalon@gmail.com</t>
   </si>
   <si>
     <t>MyMail.tls</t>
@@ -95,7 +96,7 @@
     <t>MyMail.username</t>
   </si>
   <si>
-    <t>nexi.mailin.ator@gmail.com</t>
+    <t>crypt:4556e48e5758ca346177eb5388683d5433f53d87ee3eb4f2c2de79d7bf2c2661443cb2e9d5884c8f</t>
   </si>
   <si>
     <t>MyMail.password</t>
@@ -104,6 +105,12 @@
     <t>crypt:098cc502c41d1bc8350b879974012cbe4e7ee5045dc8af70</t>
   </si>
   <si>
+    <t>MyMail.X-Mailer</t>
+  </si>
+  <si>
+    <t>nexial</t>
+  </si>
+  <si>
     <t>webmail.provider</t>
   </si>
   <si>
@@ -114,6 +121,24 @@
   </si>
   <si>
     <t>3</t>
+  </si>
+  <si>
+    <t>webmail2.provider</t>
+  </si>
+  <si>
+    <t>temporary-mail</t>
+  </si>
+  <si>
+    <t>webmail2.domain</t>
+  </si>
+  <si>
+    <t>temporary-mail.net</t>
+  </si>
+  <si>
+    <t>webmail2.inbox</t>
+  </si>
+  <si>
+    <t>deathstar852</t>
   </si>
 </sst>
 </file>
@@ -123,10 +148,10 @@
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="24">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -152,20 +177,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -174,6 +185,21 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -181,8 +207,15 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -197,29 +230,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -234,16 +252,16 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -257,16 +275,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -279,8 +305,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -295,175 +336,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -513,11 +554,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -546,17 +593,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -572,17 +608,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -601,147 +633,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="49">
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -766,7 +813,7 @@
       <protection locked="0"/>
     </xf>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -774,46 +821,48 @@
     <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
     <cellStyle name="Currency" xfId="5" builtinId="4"/>
     <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Check Cell" xfId="8" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="9" builtinId="17"/>
-    <cellStyle name="Note" xfId="10" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="11" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="12" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="13" builtinId="35"/>
-    <cellStyle name="Title" xfId="14" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="15" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="16" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="17" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="18" builtinId="19"/>
-    <cellStyle name="Input" xfId="19" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="20" builtinId="40"/>
-    <cellStyle name="Good" xfId="21" builtinId="26"/>
-    <cellStyle name="Output" xfId="22" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="23" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="24" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="25" builtinId="24"/>
-    <cellStyle name="Total" xfId="26" builtinId="25"/>
-    <cellStyle name="Bad" xfId="27" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="28" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="29" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="30" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="31" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="32" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="33" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="34" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="35" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="36" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="37" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="38" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="39" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="40" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="42" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="43" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="44" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="45" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="46" builtinId="52"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -1176,8 +1225,8 @@
   <sheetPr/>
   <dimension ref="A1:B99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16.5" outlineLevelCol="1"/>
@@ -1228,29 +1277,69 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A6" s="4"/>
-    </row>
-    <row r="7" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A7" s="4"/>
-    </row>
-    <row r="8" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A8" s="4"/>
-    </row>
-    <row r="9" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A9" s="4"/>
-    </row>
-    <row r="10" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A10" s="4"/>
-    </row>
-    <row r="11" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A11" s="4"/>
-    </row>
-    <row r="12" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A12" s="4"/>
-    </row>
-    <row r="13" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A13" s="4"/>
+    <row r="6" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="14" ht="23.1" customHeight="1" spans="1:1">
       <c r="A14" s="4"/>
@@ -1543,10 +1632,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B98"/>
+  <dimension ref="A1:B91"/>
   <sheetViews>
     <sheetView zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16.5" outlineLevelCol="1"/>
@@ -1559,75 +1648,380 @@
   <sheetData>
     <row r="1" ht="23.1" customHeight="1" spans="1:2">
       <c r="A1" s="4" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" ht="23.1" customHeight="1" spans="1:2">
       <c r="A2" s="4" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A3" s="4"/>
+    </row>
+    <row r="4" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A4" s="4"/>
+    </row>
+    <row r="5" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A5" s="4"/>
+    </row>
+    <row r="6" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A6" s="4"/>
+    </row>
+    <row r="7" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A7" s="4"/>
+    </row>
+    <row r="8" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A8" s="4"/>
+    </row>
+    <row r="9" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A9" s="4"/>
+    </row>
+    <row r="10" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A10" s="4"/>
+    </row>
+    <row r="11" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A11" s="4"/>
+    </row>
+    <row r="12" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A12" s="4"/>
+    </row>
+    <row r="13" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A13" s="4"/>
+    </row>
+    <row r="14" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A14" s="4"/>
+    </row>
+    <row r="15" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A15" s="4"/>
+    </row>
+    <row r="16" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A16" s="4"/>
+    </row>
+    <row r="17" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A17" s="4"/>
+    </row>
+    <row r="18" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A18" s="4"/>
+    </row>
+    <row r="19" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A19" s="4"/>
+    </row>
+    <row r="20" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A20" s="4"/>
+    </row>
+    <row r="21" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A21" s="4"/>
+    </row>
+    <row r="22" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A22" s="4"/>
+    </row>
+    <row r="23" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A23" s="4"/>
+    </row>
+    <row r="24" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A24" s="4"/>
+    </row>
+    <row r="25" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A25" s="4"/>
+    </row>
+    <row r="26" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A26" s="4"/>
+    </row>
+    <row r="27" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A27" s="4"/>
+    </row>
+    <row r="28" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A28" s="4"/>
+    </row>
+    <row r="29" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A29" s="4"/>
+    </row>
+    <row r="30" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A30" s="4"/>
+    </row>
+    <row r="31" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A31" s="4"/>
+    </row>
+    <row r="32" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A32" s="4"/>
+    </row>
+    <row r="33" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A33" s="4"/>
+    </row>
+    <row r="34" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A34" s="4"/>
+    </row>
+    <row r="35" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A35" s="4"/>
+    </row>
+    <row r="36" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A36" s="4"/>
+    </row>
+    <row r="37" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A37" s="4"/>
+    </row>
+    <row r="38" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A38" s="4"/>
+    </row>
+    <row r="39" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A39" s="4"/>
+    </row>
+    <row r="40" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A40" s="4"/>
+    </row>
+    <row r="41" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A41" s="4"/>
+    </row>
+    <row r="42" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A42" s="4"/>
+    </row>
+    <row r="43" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A43" s="4"/>
+    </row>
+    <row r="44" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A44" s="4"/>
+    </row>
+    <row r="45" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A45" s="4"/>
+    </row>
+    <row r="46" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A46" s="4"/>
+    </row>
+    <row r="47" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A47" s="4"/>
+    </row>
+    <row r="48" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A48" s="4"/>
+    </row>
+    <row r="49" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A49" s="4"/>
+    </row>
+    <row r="50" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A50" s="4"/>
+    </row>
+    <row r="51" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A51" s="4"/>
+    </row>
+    <row r="52" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A52" s="4"/>
+    </row>
+    <row r="53" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A53" s="4"/>
+    </row>
+    <row r="54" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A54" s="4"/>
+    </row>
+    <row r="55" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A55" s="4"/>
+    </row>
+    <row r="56" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A56" s="4"/>
+    </row>
+    <row r="57" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A57" s="4"/>
+    </row>
+    <row r="58" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A58" s="4"/>
+    </row>
+    <row r="59" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A59" s="4"/>
+    </row>
+    <row r="60" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A60" s="4"/>
+    </row>
+    <row r="61" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A61" s="4"/>
+    </row>
+    <row r="62" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A62" s="4"/>
+    </row>
+    <row r="63" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A63" s="4"/>
+    </row>
+    <row r="64" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A64" s="4"/>
+    </row>
+    <row r="65" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A65" s="4"/>
+    </row>
+    <row r="66" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A66" s="4"/>
+    </row>
+    <row r="67" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A67" s="4"/>
+    </row>
+    <row r="68" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A68" s="4"/>
+    </row>
+    <row r="69" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A69" s="4"/>
+    </row>
+    <row r="70" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A70" s="4"/>
+    </row>
+    <row r="71" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A71" s="4"/>
+    </row>
+    <row r="72" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A72" s="4"/>
+    </row>
+    <row r="73" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A73" s="4"/>
+    </row>
+    <row r="74" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A74" s="4"/>
+    </row>
+    <row r="75" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A75" s="4"/>
+    </row>
+    <row r="76" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A76" s="4"/>
+    </row>
+    <row r="77" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A77" s="4"/>
+    </row>
+    <row r="78" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A78" s="4"/>
+    </row>
+    <row r="79" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A79" s="4"/>
+    </row>
+    <row r="80" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A80" s="4"/>
+    </row>
+    <row r="81" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A81" s="4"/>
+    </row>
+    <row r="82" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A82" s="4"/>
+    </row>
+    <row r="83" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A83" s="4"/>
+    </row>
+    <row r="84" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A84" s="4"/>
+    </row>
+    <row r="85" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A85" s="4"/>
+    </row>
+    <row r="86" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A86" s="4"/>
+    </row>
+    <row r="87" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A87" s="4"/>
+    </row>
+    <row r="88" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A88" s="4"/>
+    </row>
+    <row r="89" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A89" s="4"/>
+    </row>
+    <row r="90" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A90" s="4"/>
+    </row>
+    <row r="91" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A91" s="4"/>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" deleteColumns="0" deleteRows="0" sort="0"/>
+  <conditionalFormatting sqref="A$1:A$1048576">
+    <cfRule type="beginsWith" dxfId="0" priority="1" stopIfTrue="1" operator="equal" text="//">
+      <formula>LEFT(A1,LEN("//"))="//"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="2" stopIfTrue="1" operator="equal" text="nexial.scope.">
+      <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="3" stopIfTrue="1" operator="equal" text="nexial.">
+      <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="3" priority="4" stopIfTrue="1">
+      <formula>LEN(TRIM(A1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B$1:E$1048576">
+    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="5" priority="6">
+      <formula>LEN(TRIM(B1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B93"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16.5" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="15.8" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.8" style="2" customWidth="1"/>
+    <col min="3" max="5" width="21.3" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="10.7" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="3" ht="23.1" customHeight="1" spans="1:2">
       <c r="A3" s="4" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" ht="23.1" customHeight="1" spans="1:2">
       <c r="A4" s="4" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" ht="23.1" customHeight="1" spans="1:2">
-      <c r="A9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>25</v>
-      </c>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A5" s="4"/>
+    </row>
+    <row r="6" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A6" s="4"/>
+    </row>
+    <row r="7" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A7" s="4"/>
+    </row>
+    <row r="8" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A8" s="4"/>
+    </row>
+    <row r="9" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A9" s="4"/>
     </row>
     <row r="10" ht="23.1" customHeight="1" spans="1:1">
       <c r="A10" s="4"/>
@@ -1880,21 +2274,6 @@
     </row>
     <row r="93" ht="23.1" customHeight="1" spans="1:1">
       <c r="A93" s="4"/>
-    </row>
-    <row r="94" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A94" s="4"/>
-    </row>
-    <row r="95" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A95" s="4"/>
-    </row>
-    <row r="96" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A96" s="4"/>
-    </row>
-    <row r="97" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A97" s="4"/>
-    </row>
-    <row r="98" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A98" s="4"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" deleteColumns="0" deleteRows="0" sort="0"/>

</xml_diff>

<commit_message>
[mobile] - automatically add [`scenarioRef`](../systemvars/index.html#nexial.scenarioRef) for the mobile device used in automation.
Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/data/unitTest_webmail.data.xlsx
+++ b/src/test/resources/unittesting/artifact/data/unitTest_webmail.data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="12645" tabRatio="500" activeTab="2"/>
+    <workbookView windowWidth="28800" windowHeight="11610" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -60,7 +60,7 @@
     <t>nexial.browser</t>
   </si>
   <si>
-    <t>chrome</t>
+    <t>chrome.headless</t>
   </si>
   <si>
     <t>nexial.web.pageLoadWaitMs</t>
@@ -146,9 +146,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="24">
@@ -177,9 +177,31 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -191,8 +213,47 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -206,38 +267,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -252,61 +283,15 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -321,7 +306,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -336,73 +336,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -414,109 +510,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -545,15 +545,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -571,8 +562,10 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -589,6 +582,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -610,11 +612,18 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -633,162 +642,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1225,8 +1225,8 @@
   <sheetPr/>
   <dimension ref="A1:B99"/>
   <sheetViews>
-    <sheetView zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16.5" outlineLevelCol="1"/>
@@ -1964,8 +1964,8 @@
   <sheetPr/>
   <dimension ref="A1:B93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16.5" outlineLevelCol="1"/>

</xml_diff>

<commit_message>
update unit test for webmail
Signed-off-by: automike <mike.liu@covetrus.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/data/unitTest_webmail.data.xlsx
+++ b/src/test/resources/unittesting/artifact/data/unitTest_webmail.data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11610" tabRatio="500"/>
+    <workbookView windowWidth="28125" windowHeight="13080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -72,7 +72,7 @@
     <t>MyMail.host</t>
   </si>
   <si>
-    <t>smtp.gmail.com</t>
+    <t>crypt:361cbccaab164a3c714b216e6856de939de18c49c0d977db4cf6b337db7c89a4</t>
   </si>
   <si>
     <t>MyMail.port</t>
@@ -84,7 +84,7 @@
     <t>MyMail.from</t>
   </si>
   <si>
-    <t>jimmyfalon@gmail.com</t>
+    <t>crypt:952650272c296d08a78b9588b6dbcbe1c4e458189fd9cb851a95388fb3edb636</t>
   </si>
   <si>
     <t>MyMail.tls</t>
@@ -96,13 +96,13 @@
     <t>MyMail.username</t>
   </si>
   <si>
-    <t>crypt:4556e48e5758ca346177eb5388683d5433f53d87ee3eb4f2c2de79d7bf2c2661443cb2e9d5884c8f</t>
+    <t>crypt:1358294330ca2abd0c3dd34251d0645ef7f520075db06ff3e7d2bcd8e64f6fb6</t>
   </si>
   <si>
     <t>MyMail.password</t>
   </si>
   <si>
-    <t>crypt:098cc502c41d1bc8350b879974012cbe4e7ee5045dc8af70</t>
+    <t>crypt:91d32852b47c9e466e79df6e9521f7f0e9bf3ca7495a6c06</t>
   </si>
   <si>
     <t>MyMail.X-Mailer</t>
@@ -146,10 +146,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -179,6 +179,20 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -190,55 +204,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -253,30 +221,31 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -291,17 +260,10 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -314,7 +276,45 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -336,19 +336,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -360,163 +510,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -546,6 +546,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -560,13 +575,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -595,17 +614,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -621,24 +634,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -647,148 +647,148 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1226,7 +1226,7 @@
   <dimension ref="A1:B99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16.5" outlineLevelCol="1"/>

</xml_diff>

<commit_message>
- fixing unit test on webmail
Signed-off-by: automike <mike.liu@covetrus.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/data/unitTest_webmail.data.xlsx
+++ b/src/test/resources/unittesting/artifact/data/unitTest_webmail.data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="13080" tabRatio="500"/>
+    <workbookView windowHeight="13080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t>nexial.scope.fallbackToPrevious</t>
   </si>
@@ -72,7 +72,7 @@
     <t>MyMail.host</t>
   </si>
   <si>
-    <t>crypt:36eab3c8db50fe57796eaa76ee378b96981ed14d644986d4db92003e1df0fb6c</t>
+    <t>crypt:4e48a099c8a6be4c47ed42cd88d251c9aa022e006445dd6c4d46bc7050e3355539399a74d3ceb9f5</t>
   </si>
   <si>
     <t>MyMail.port</t>
@@ -84,7 +84,7 @@
     <t>MyMail.from</t>
   </si>
   <si>
-    <t>crypt:952650272c296d08a78b9588b6dbcbe1c4e458189fd9cb851a95388fb3edb636</t>
+    <t>crypt:4f1b8b0828f08358bb833294b17931fda6f82b3c30861a31eb9ad03ad17f5ecc</t>
   </si>
   <si>
     <t>MyMail.tls</t>
@@ -96,19 +96,49 @@
     <t>MyMail.username</t>
   </si>
   <si>
-    <t>crypt:1358294330ca2abd0c3dd34251d0645ef7f520075db06ff3e7d2bcd8e64f6fb6</t>
+    <t>crypt:307d6c3244b56794b178c0d265d95a5a378b1ebfea023b3ab9a5bd2d48a2bd27</t>
   </si>
   <si>
     <t>MyMail.password</t>
   </si>
   <si>
-    <t>crypt:91d32852b47c9e466e79df6e9521f7f0e9bf3ca7495a6c06</t>
+    <t>crypt:a8259ea7c09e8b47a8386ad4a41691b755e83867b0af88fa07d412f8b41223ec</t>
   </si>
   <si>
     <t>MyMail.X-Mailer</t>
   </si>
   <si>
     <t>nexial</t>
+  </si>
+  <si>
+    <t>sib.key</t>
+  </si>
+  <si>
+    <t>crypt:b9c6affefc191f88b74f13bcac3636e5ff6be6cdaca5b821a91c099b416fa427d3d744df524492cbf78de2029f91fad6305322194e070b6a28b8aab9fdd3f5bce36cca336d1b7c797c90d391834898d5f42b37d6a67b732a13e03227f2db7333cfa1604ec77499d2</t>
+  </si>
+  <si>
+    <t>sib.url</t>
+  </si>
+  <si>
+    <t>crypt:a2c99e1549a2da056b78cc4d3345d770851c3f85a0666510432cf17655444f675afba4fe4da545feb65efc42818033b7fc6e947eb0999ccd</t>
+  </si>
+  <si>
+    <t>sib.sender</t>
+  </si>
+  <si>
+    <t>crypt:262a2cb2b0b479bf4b59d1fc8d86e345354972a0bb047da13508bfbb5da2e412</t>
+  </si>
+  <si>
+    <t>sib.replyTo</t>
+  </si>
+  <si>
+    <t>${sib.sender}</t>
+  </si>
+  <si>
+    <t>sib.email.template</t>
+  </si>
+  <si>
+    <t>$(syspath|data|fullpath)/unitTest_webmail.mail.template.json</t>
   </si>
   <si>
     <t>webmail.provider</t>
@@ -146,10 +176,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -176,16 +206,24 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -199,23 +237,46 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -229,31 +290,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -261,14 +315,6 @@
     <font>
       <b/>
       <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -289,17 +335,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -314,13 +351,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -336,13 +366,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -354,169 +528,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -545,26 +575,32 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -584,21 +620,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -611,23 +632,32 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -647,148 +677,148 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1223,10 +1253,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B99"/>
+  <dimension ref="A1:B101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16.5" outlineLevelCol="1"/>
@@ -1341,20 +1371,45 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A14" s="4"/>
-    </row>
-    <row r="15" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A15" s="4"/>
-    </row>
-    <row r="16" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A16" s="4"/>
-    </row>
-    <row r="17" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A17" s="4"/>
-    </row>
-    <row r="18" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A18" s="4"/>
+    <row r="14" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A17" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A18" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="19" ht="23.1" customHeight="1" spans="1:1">
       <c r="A19" s="4"/>
@@ -1598,6 +1653,12 @@
     </row>
     <row r="99" ht="23.1" customHeight="1" spans="1:1">
       <c r="A99" s="4"/>
+    </row>
+    <row r="100" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A100" s="4"/>
+    </row>
+    <row r="101" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A101" s="4"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" deleteColumns="0" deleteRows="0" sort="0"/>
@@ -1648,18 +1709,18 @@
   <sheetData>
     <row r="1" ht="23.1" customHeight="1" spans="1:2">
       <c r="A1" s="4" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" ht="23.1" customHeight="1" spans="1:2">
       <c r="A2" s="4" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" ht="23.1" customHeight="1" spans="1:1">
@@ -1965,7 +2026,7 @@
   <dimension ref="A1:B93"/>
   <sheetViews>
     <sheetView zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16.5" outlineLevelCol="1"/>
@@ -1978,34 +2039,34 @@
   <sheetData>
     <row r="1" ht="23.1" customHeight="1" spans="1:2">
       <c r="A1" s="4" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" ht="23.1" customHeight="1" spans="1:2">
       <c r="A2" s="4" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" ht="23.1" customHeight="1" spans="1:2">
       <c r="A3" s="4" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" ht="23.1" customHeight="1" spans="1:2">
       <c r="A4" s="4" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" ht="23.1" customHeight="1" spans="1:1">

</xml_diff>

<commit_message>
[improvements] - enforce Java 17 as the minimum required Java version; helps to improve runtime stability and performance, and enable future enhancements   - also upgrade to Kotlin v1.7, Gradle v7.x
- update build.gradle:
  - update a bunch of 3rd party libraries
  - set test parallelism to 10
  - added `add-exports` to test task
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/data/unitTest_webmail.data.xlsx
+++ b/src/test/resources/unittesting/artifact/data/unitTest_webmail.data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="13080" tabRatio="500"/>
+    <workbookView windowHeight="16700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>nexial.scope.fallbackToPrevious</t>
   </si>
@@ -72,7 +72,7 @@
     <t>MyMail.host</t>
   </si>
   <si>
-    <t>crypt:4e48a099c8a6be4c47ed42cd88d251c9aa022e006445dd6c4d46bc7050e3355539399a74d3ceb9f5</t>
+    <t>smtp.gmail.com</t>
   </si>
   <si>
     <t>MyMail.port</t>
@@ -84,7 +84,7 @@
     <t>MyMail.from</t>
   </si>
   <si>
-    <t>crypt:4f1b8b0828f08358bb833294b17931fda6f82b3c30861a31eb9ad03ad17f5ecc</t>
+    <t>nexial-no-reply@accionlabs.com</t>
   </si>
   <si>
     <t>MyMail.tls</t>
@@ -96,13 +96,10 @@
     <t>MyMail.username</t>
   </si>
   <si>
-    <t>crypt:307d6c3244b56794b178c0d265d95a5a378b1ebfea023b3ab9a5bd2d48a2bd27</t>
-  </si>
-  <si>
     <t>MyMail.password</t>
   </si>
   <si>
-    <t>crypt:a8259ea7c09e8b47a8386ad4a41691b755e83867b0af88fa07d412f8b41223ec</t>
+    <t>n3x1*!-n0_r@ply!!</t>
   </si>
   <si>
     <t>MyMail.X-Mailer</t>
@@ -176,9 +173,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
@@ -208,14 +205,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -223,7 +213,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -231,6 +221,59 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -245,98 +288,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -356,6 +307,52 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -366,19 +363,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -390,163 +543,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -575,17 +572,35 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -605,6 +620,41 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -619,210 +669,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -842,57 +839,64 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
     <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -1256,15 +1260,15 @@
   <dimension ref="A1:B101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16.5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="10.7013888888889" defaultRowHeight="14.4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="23.9" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.3" style="2" customWidth="1"/>
-    <col min="3" max="5" width="21.3" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="10.7" style="3"/>
+    <col min="1" max="1" width="23.9027777777778" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.2986111111111" style="2" customWidth="1"/>
+    <col min="3" max="5" width="21.2986111111111" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="10.7013888888889" style="3"/>
   </cols>
   <sheetData>
     <row r="1" ht="23.1" customHeight="1" spans="1:2">
@@ -1327,7 +1331,7 @@
       <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="5" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1351,64 +1355,64 @@
       <c r="A11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>19</v>
+      <c r="B11" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="12" ht="23.1" customHeight="1" spans="1:2">
       <c r="A12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="13" ht="23.1" customHeight="1" spans="1:2">
       <c r="A13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="14" ht="23.1" customHeight="1" spans="1:2">
       <c r="A14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="15" ht="23.1" customHeight="1" spans="1:2">
       <c r="A15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="16" ht="23.1" customHeight="1" spans="1:2">
       <c r="A16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="17" ht="23.1" customHeight="1" spans="1:2">
       <c r="A17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="18" ht="23.1" customHeight="1" spans="1:2">
       <c r="A18" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="19" ht="23.1" customHeight="1" spans="1:1">
@@ -1676,7 +1680,7 @@
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B$1:E$1048576">
+  <conditionalFormatting sqref="B1:E7 C8:E8 B9:E10 C11:E11 B12:E1048576">
     <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
@@ -1684,6 +1688,10 @@
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="B8" r:id="rId1" display="nexial-no-reply@accionlabs.com"/>
+    <hyperlink ref="B11" r:id="rId1" display="nexial-no-reply@accionlabs.com"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>
   <headerFooter/>
@@ -1699,28 +1707,28 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16.5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="10.7013888888889" defaultRowHeight="14.4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="15.8" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.8" style="2" customWidth="1"/>
-    <col min="3" max="5" width="21.3" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="10.7" style="3"/>
+    <col min="1" max="1" width="15.7986111111111" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7986111111111" style="2" customWidth="1"/>
+    <col min="3" max="5" width="21.2986111111111" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="10.7013888888889" style="3"/>
   </cols>
   <sheetData>
     <row r="1" ht="23.1" customHeight="1" spans="1:2">
       <c r="A1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" ht="23.1" customHeight="1" spans="1:2">
       <c r="A2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="3" ht="23.1" customHeight="1" spans="1:1">
@@ -2026,47 +2034,47 @@
   <dimension ref="A1:B93"/>
   <sheetViews>
     <sheetView zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16.5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="10.7013888888889" defaultRowHeight="14.4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="15.8" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.8" style="2" customWidth="1"/>
-    <col min="3" max="5" width="21.3" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="10.7" style="3"/>
+    <col min="1" max="1" width="15.7986111111111" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7986111111111" style="2" customWidth="1"/>
+    <col min="3" max="5" width="21.2986111111111" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="10.7013888888889" style="3"/>
   </cols>
   <sheetData>
     <row r="1" ht="23.1" customHeight="1" spans="1:2">
       <c r="A1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" ht="23.1" customHeight="1" spans="1:2">
       <c r="A2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="3" ht="23.1" customHeight="1" spans="1:2">
       <c r="A3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="4" ht="23.1" customHeight="1" spans="1:2">
       <c r="A4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="5" ht="23.1" customHeight="1" spans="1:1">

</xml_diff>

<commit_message>
Nexial 4.6 - minor tweak to jenkins-related styling - updated 3rd party library (xalan) - updated code to Java 17 syntax (more to come...)
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/data/unitTest_webmail.data.xlsx
+++ b/src/test/resources/unittesting/artifact/data/unitTest_webmail.data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="25180" tabRatio="500"/>
+    <workbookView windowHeight="27260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -102,7 +102,7 @@
     <t>MyMail.password</t>
   </si>
   <si>
-    <t>crypt:15a6e17be5df352d19b07f02e75a0fcf6685e1ba7baeed87f05c392d64d5016a</t>
+    <t>crypt:f3ad36f43d15999c9bc03d24f66918cfcb12e6b011ab65d4a479f2c7386b4f61</t>
   </si>
   <si>
     <t>MyMail.X-Mailer</t>
@@ -179,10 +179,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -209,6 +209,14 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -217,10 +225,17 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -240,22 +255,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -277,33 +277,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -322,24 +307,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -354,7 +332,29 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -369,31 +369,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -405,145 +543,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -578,6 +578,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -587,11 +602,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -611,32 +647,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -644,8 +659,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -660,172 +675,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -849,6 +849,10 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1266,7 +1270,7 @@
   <dimension ref="A1:B102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7013888888889" defaultRowHeight="14.4" outlineLevelCol="1"/>
@@ -1377,7 +1381,7 @@
       <c r="A13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="7" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2047,7 +2051,7 @@
   <dimension ref="A1:B93"/>
   <sheetViews>
     <sheetView zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7013888888889" defaultRowHeight="14.4" outlineLevelCol="1"/>

</xml_diff>